<commit_message>
bump to .net 6.0, bump all packages to newest version
</commit_message>
<xml_diff>
--- a/Features.xlsx
+++ b/Features.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Develop\Extern\GitHub.KsWare\AppVeyorClient\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B999D943-1D85-4E82-90A8-1FB8318C3EEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2187CA48-EE6D-4482-B897-616736D2AD7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2292" yWindow="-108" windowWidth="28536" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="33">
   <si>
     <t>Menu</t>
   </si>
@@ -117,10 +117,13 @@
     <t>obsolete</t>
   </si>
   <si>
-    <t>outsource KsWare.AppVerrior.Api</t>
-  </si>
-  <si>
     <t>Encrypt values</t>
+  </si>
+  <si>
+    <t>Validate yaml</t>
+  </si>
+  <si>
+    <t>outsource KsWare.AppVeyor.Api</t>
   </si>
 </sst>
 </file>
@@ -508,7 +511,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:C26"/>
+  <dimension ref="A3:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A26" sqref="A26"/>
@@ -597,6 +600,12 @@
       <c r="A11" t="s">
         <v>7</v>
       </c>
+      <c r="B11" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -743,7 +752,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>3</v>
@@ -754,12 +763,23 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C26" t="s">
+      <c r="B27" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>